<commit_message>
Fix Bugs in Check package
</commit_message>
<xml_diff>
--- a/data-raw/Daten_Beispiel.xlsx
+++ b/data-raw/Daten_Beispiel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="23280" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Daten_Beispiel" sheetId="1" r:id="rId1"/>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +473,7 @@
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -522,11 +522,11 @@
       <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -579,12 +579,12 @@
         <f>G2</f>
         <v>36</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <f>SUM(C2,F2)</f>
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -637,12 +637,12 @@
         <f t="shared" ref="P3:P4" si="3">G3</f>
         <v>13</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R15" si="4">SUM(C3,F3)</f>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q15" si="4">SUM(C3,F3)</f>
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -695,12 +695,12 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="R4">
+      <c r="Q4">
         <f t="shared" si="4"/>
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -749,12 +749,12 @@
       <c r="P5">
         <v>196</v>
       </c>
-      <c r="R5">
+      <c r="Q5">
         <f t="shared" si="4"/>
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -807,12 +807,12 @@
         <f>G6</f>
         <v>35</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <f t="shared" si="4"/>
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -861,12 +861,12 @@
       <c r="P7">
         <v>69</v>
       </c>
-      <c r="R7">
+      <c r="Q7">
         <f t="shared" si="4"/>
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -919,12 +919,12 @@
         <f>G8</f>
         <v>19</v>
       </c>
-      <c r="R8">
+      <c r="Q8">
         <f t="shared" si="4"/>
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -973,12 +973,12 @@
       <c r="P9">
         <v>49</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1027,12 +1027,12 @@
       <c r="P10">
         <v>5</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1081,12 +1081,12 @@
       <c r="P11">
         <v>50</v>
       </c>
-      <c r="R11">
+      <c r="Q11">
         <f t="shared" si="4"/>
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1135,12 +1135,12 @@
       <c r="P12">
         <v>10</v>
       </c>
-      <c r="R12">
+      <c r="Q12">
         <f t="shared" si="4"/>
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1193,12 +1193,12 @@
         <f>G13</f>
         <v>67</v>
       </c>
-      <c r="R13">
+      <c r="Q13">
         <f t="shared" si="4"/>
         <v>256</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1251,12 +1251,12 @@
         <f>G14</f>
         <v>15</v>
       </c>
-      <c r="R14">
+      <c r="Q14">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="P15">
         <v>112</v>
       </c>
-      <c r="R15">
+      <c r="Q15">
         <f t="shared" si="4"/>
         <v>419</v>
       </c>

</xml_diff>